<commit_message>
dataset size incresed to 1000 imgs for better results
</commit_message>
<xml_diff>
--- a/Attendance_Log.xlsx
+++ b/Attendance_Log.xlsx
@@ -15,7 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Arial"/>
@@ -44,8 +46,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -324,7 +327,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -335,13 +338,16 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Shyam</t>
+          <t>Bharat</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Present</t>
+          <t>Absent</t>
         </is>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>45480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>